<commit_message>
Starting on ubuntu OS
</commit_message>
<xml_diff>
--- a/transactions2.xlsx
+++ b/transactions2.xlsx
@@ -1,47 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price </t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00"/>
+    <numFmt formatCode="[$$-C09]#,##0.00;[RED]\-[$$-C09]#,##0.00" numFmtId="164"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,19 +58,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -356,77 +378,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100">
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125" style="1" customWidth="1"/>
+    <col customWidth="1" max="1025" min="1" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row customHeight="1" ht="12.8" r="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>transaction_id</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">price </t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="2" s="3">
+      <c r="A2" s="2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="4" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.355</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="3">
+      <c r="A3" s="2" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="C3" s="4" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6.255</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="1">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5.95</v>
-      </c>
-      <c r="D2">
-        <v>5.3550000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A3" s="1">
-        <v>1002</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>6.95</v>
-      </c>
-      <c r="D3">
-        <v>6.2549999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A4" s="1">
+    <row customHeight="1" ht="12.8" r="4" s="3">
+      <c r="A4" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4" t="n">
         <v>7.95</v>
       </c>
-      <c r="D4">
-        <v>7.1550000000000002</v>
+      <c r="D4" t="n">
+        <v>7.155</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>